<commit_message>
Algemeen tijdschrijf formulier :dog:
</commit_message>
<xml_diff>
--- a/Docs/tijd_schrijven/Tijdschrijfformulier.xlsx
+++ b/Docs/tijd_schrijven/Tijdschrijfformulier.xlsx
@@ -5,26 +5,26 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jochem\Documents\Actual Documents\School\HBO Windesheim ICT\Klas 1\nerdy_gadgets\Docs\tijd_schrijven\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\NerdyGadgets\Docs\tijd_schrijven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DBDBAE-9D3F-45A0-9DBB-28438A81FBB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9C37F0-1F00-43AE-9A08-D29AA9DBE0D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Projectlid1" sheetId="7" r:id="rId1"/>
-    <sheet name="Projectlid2" sheetId="8" r:id="rId2"/>
-    <sheet name="Projectlid3" sheetId="9" r:id="rId3"/>
-    <sheet name="Projectlid4" sheetId="10" r:id="rId4"/>
-    <sheet name="Projectlid5" sheetId="11" r:id="rId5"/>
+    <sheet name="Marvin" sheetId="7" r:id="rId1"/>
+    <sheet name="Demi" sheetId="8" r:id="rId2"/>
+    <sheet name="Lucas" sheetId="9" r:id="rId3"/>
+    <sheet name="Luuk" sheetId="10" r:id="rId4"/>
+    <sheet name="Joch" sheetId="11" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Projectlid1!$A$1:$D$47</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Projectlid2!$A$1:$D$47</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">Projectlid3!$A$1:$D$47</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">Projectlid4!$A$1:$D$47</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">Projectlid5!$A$1:$D$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Demi!$A$1:$D$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">Joch!$A$1:$D$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">Lucas!$A$1:$D$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">Luuk!$A$1:$D$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Marvin!$A$1:$D$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="27">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -114,6 +114,18 @@
   </si>
   <si>
     <t>Thuis tijdens de les</t>
+  </si>
+  <si>
+    <t>Werken buiten school</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Werken buiten school </t>
+  </si>
+  <si>
+    <t>thuis werken tijdens en na les</t>
+  </si>
+  <si>
+    <t>Online werken tijdens les</t>
   </si>
 </sst>
 </file>
@@ -566,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="B2" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,7 +632,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -632,7 +644,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -698,8 +710,17 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
       <c r="B13" s="2">
         <v>45243</v>
+      </c>
+      <c r="C13">
+        <v>120</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -728,7 +749,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="B2" sqref="B1:B1048576"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,7 +802,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -793,7 +814,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -859,8 +880,17 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
       <c r="B13" s="2">
         <v>45243</v>
+      </c>
+      <c r="C13">
+        <v>120</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -889,7 +919,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="B2" sqref="B1:B1048576"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,7 +972,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -954,7 +984,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1020,8 +1050,17 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
       <c r="B13" s="2">
         <v>45243</v>
+      </c>
+      <c r="C13">
+        <v>120</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1049,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,7 +1142,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>6</v>
+        <v>10.666666666666666</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1115,7 +1154,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>162</v>
+        <v>157.33333333333334</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1181,8 +1220,17 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
       <c r="B13" s="2">
         <v>45243</v>
+      </c>
+      <c r="C13">
+        <v>280</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1211,7 +1259,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B13"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,7 +1312,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>10</v>
+        <v>10.666666666666666</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1276,7 +1324,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>158</v>
+        <v>157.33333333333334</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1349,7 +1397,7 @@
         <v>45243</v>
       </c>
       <c r="C13">
-        <v>240</v>
+        <v>280</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
@@ -1378,6 +1426,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="e39e5be6c3b6c984bf8187e86b359ac0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ced390a3fc2668719c5d57d8ce08db4" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1603,26 +1670,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAC8759-EB35-489F-BF7F-6A43D48E2DBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1640,30 +1714,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>